<commit_message>
fix bugs associated with adding samples to spawnings
</commit_message>
<xml_diff>
--- a/bio_diversity/static/data_templates/coldbrook-spawning.xlsx
+++ b/bio_diversity/static/data_templates/coldbrook-spawning.xlsx
@@ -91,11 +91,25 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
+          <t>Optional, must match exisiting sample number.
+PIT tag field must be blank.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G3" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
           <t>Priority of Female: H/M/L/P</t>
         </r>
       </text>
     </comment>
-    <comment ref="G3" authorId="1" shapeId="0">
+    <comment ref="H3" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -119,7 +133,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H3" authorId="1" shapeId="0">
+    <comment ref="I3" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -132,7 +146,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I3" authorId="1" shapeId="0">
+    <comment ref="J3" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -145,7 +159,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J3" authorId="1" shapeId="0">
+    <comment ref="K3" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -159,7 +173,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K3" authorId="1" shapeId="0">
+    <comment ref="L3" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -173,7 +187,21 @@
         </r>
       </text>
     </comment>
-    <comment ref="M3" authorId="1" shapeId="0">
+    <comment ref="N3" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Optional, must match exisiting sample number.
+PIT tag field must be blank.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O3" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -186,7 +214,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N3" authorId="1" shapeId="0">
+    <comment ref="P3" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -199,7 +227,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O3" authorId="1" shapeId="0">
+    <comment ref="Q3" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -212,7 +240,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P3" authorId="1" shapeId="0">
+    <comment ref="R3" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -225,7 +253,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q3" authorId="1" shapeId="0">
+    <comment ref="S3" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -238,7 +266,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R3" authorId="1" shapeId="0">
+    <comment ref="T3" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -252,7 +280,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S3" authorId="1" shapeId="0">
+    <comment ref="U3" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -267,7 +295,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T3" authorId="1" shapeId="0">
+    <comment ref="V3" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -281,7 +309,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U3" authorId="1" shapeId="0">
+    <comment ref="W3" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -294,7 +322,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V3" authorId="1" shapeId="0">
+    <comment ref="X3" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -307,7 +335,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W3" authorId="1" shapeId="0">
+    <comment ref="Y3" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -325,7 +353,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Year</t>
   </si>
@@ -403,6 +431,12 @@
   </si>
   <si>
     <t>Program</t>
+  </si>
+  <si>
+    <t>Sample UFID, F</t>
+  </si>
+  <si>
+    <t>Sample UFID, M</t>
   </si>
 </sst>
 </file>
@@ -814,10 +848,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:W16"/>
+  <dimension ref="A2:Y16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V3" sqref="V3"/>
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -826,48 +860,51 @@
     <col min="2" max="2" width="7.7109375" customWidth="1"/>
     <col min="3" max="3" width="4.5703125" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" customWidth="1"/>
-    <col min="8" max="8" width="11.5703125" customWidth="1"/>
-    <col min="9" max="9" width="12.7109375" customWidth="1"/>
-    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.5703125" customWidth="1"/>
-    <col min="14" max="14" width="11.42578125" customWidth="1"/>
-    <col min="15" max="15" width="11.28515625" customWidth="1"/>
-    <col min="18" max="18" width="16.7109375" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" customWidth="1"/>
+    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.5703125" customWidth="1"/>
+    <col min="16" max="16" width="11.42578125" customWidth="1"/>
+    <col min="17" max="17" width="11.28515625" customWidth="1"/>
+    <col min="20" max="20" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="6"/>
+      <c r="H2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="6"/>
       <c r="I2" s="6"/>
       <c r="J2" s="6"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="8"/>
       <c r="M2" s="6"/>
-      <c r="N2" s="7" t="s">
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
+      <c r="P2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="O2" s="6"/>
-      <c r="P2" s="6"/>
       <c r="Q2" s="6"/>
       <c r="R2" s="6"/>
-      <c r="S2" s="8"/>
+      <c r="S2" s="6"/>
       <c r="T2" s="6"/>
-      <c r="U2" s="6" t="s">
+      <c r="U2" s="8"/>
+      <c r="V2" s="6"/>
+      <c r="W2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="V2" s="6"/>
-      <c r="W2" s="6"/>
-    </row>
-    <row r="3" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="X2" s="6"/>
+      <c r="Y2" s="6"/>
+    </row>
+    <row r="3" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -883,114 +920,120 @@
       <c r="E3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="L3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="N3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="P3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="Q3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="R3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="Q3" s="2" t="s">
+      <c r="S3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="R3" s="3" t="s">
+      <c r="T3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="S3" s="9" t="s">
+      <c r="U3" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="T3" s="1" t="s">
+      <c r="V3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U3" s="1" t="s">
+      <c r="W3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="V3" s="1" t="s">
+      <c r="X3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="W3" s="1" t="s">
+      <c r="Y3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="H4" s="10"/>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="I4" s="10"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="H6" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="10"/>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="I6" s="10"/>
-      <c r="N6" s="10"/>
-      <c r="O6" s="10"/>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="H7" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="10"/>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="I7" s="10"/>
-      <c r="N7" s="10"/>
-      <c r="O7" s="10"/>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="H8" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="10"/>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="I8" s="10"/>
-      <c r="N8" s="10"/>
-      <c r="O8" s="10"/>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="H9" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="10"/>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="I9" s="10"/>
-      <c r="N9" s="10"/>
-      <c r="O9" s="10"/>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="H10" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="10"/>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="I10" s="10"/>
-      <c r="N10" s="10"/>
-      <c r="O10" s="10"/>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="J13" s="11"/>
-      <c r="K13" s="13"/>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="I14" s="14"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="15"/>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="I15" s="14"/>
-      <c r="J15" s="12"/>
-      <c r="K15" s="13"/>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="J16" s="11"/>
-      <c r="K16" s="16"/>
+      <c r="J10" s="10"/>
+      <c r="P10" s="10"/>
+      <c r="Q10" s="10"/>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="K13" s="11"/>
+      <c r="L13" s="13"/>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="J14" s="14"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="15"/>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="J15" s="14"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="13"/>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="K16" s="11"/>
+      <c r="L16" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add cryo features into spawning parsers
</commit_message>
<xml_diff>
--- a/bio_diversity/static/data_templates/coldbrook-spawning.xlsx
+++ b/bio_diversity/static/data_templates/coldbrook-spawning.xlsx
@@ -168,26 +168,52 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
+          <t>Optional, Y/N.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L3" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Optional, Y/N.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M3" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
           <t xml:space="preserve">Release / Keep
 </t>
         </r>
       </text>
     </comment>
-    <comment ref="L3" authorId="1" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Tank fish is placed in after spawning
+    <comment ref="N3" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Optional. Tank fish is placed in after spawning
 </t>
         </r>
       </text>
     </comment>
-    <comment ref="N3" authorId="1" shapeId="0">
+    <comment ref="P3" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -201,7 +227,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O3" authorId="1" shapeId="0">
+    <comment ref="Q3" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -214,7 +240,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P3" authorId="1" shapeId="0">
+    <comment ref="R3" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -227,7 +253,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q3" authorId="1" shapeId="0">
+    <comment ref="S3" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -240,7 +266,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R3" authorId="1" shapeId="0">
+    <comment ref="T3" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -253,7 +279,34 @@
         </r>
       </text>
     </comment>
-    <comment ref="S3" authorId="1" shapeId="0">
+    <comment ref="U3" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Optional, Y/N</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="V3" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <u/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Optional Y/N</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="W3" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -266,21 +319,21 @@
         </r>
       </text>
     </comment>
-    <comment ref="T3" authorId="1" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Tank fish is placed in after spawning
+    <comment ref="X3" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Optional. Tank fish is placed in after spawning
 </t>
         </r>
       </text>
     </comment>
-    <comment ref="U3" authorId="1" shapeId="0">
+    <comment ref="Y3" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -295,7 +348,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V3" authorId="1" shapeId="0">
+    <comment ref="Z3" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -309,7 +362,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W3" authorId="1" shapeId="0">
+    <comment ref="AA3" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -322,7 +375,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X3" authorId="1" shapeId="0">
+    <comment ref="AB3" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -335,7 +388,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y3" authorId="1" shapeId="0">
+    <comment ref="AC3" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -353,7 +406,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Year</t>
   </si>
@@ -437,6 +490,18 @@
   </si>
   <si>
     <t>Sample UFID, M</t>
+  </si>
+  <si>
+    <t>Ovarian Fluid Taken?</t>
+  </si>
+  <si>
+    <t>Ovarian Fluid Used</t>
+  </si>
+  <si>
+    <t>Cryo Milt Taken</t>
+  </si>
+  <si>
+    <t>Cryo Milt Used</t>
   </si>
 </sst>
 </file>
@@ -446,7 +511,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -481,6 +546,13 @@
     </font>
     <font>
       <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
@@ -848,10 +920,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:Y16"/>
+  <dimension ref="A2:AC16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+      <selection activeCell="K1" sqref="K1:L1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -864,14 +936,18 @@
     <col min="8" max="8" width="15.7109375" customWidth="1"/>
     <col min="9" max="9" width="11.5703125" customWidth="1"/>
     <col min="10" max="10" width="12.7109375" customWidth="1"/>
-    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.5703125" customWidth="1"/>
-    <col min="16" max="16" width="11.42578125" customWidth="1"/>
-    <col min="17" max="17" width="11.28515625" customWidth="1"/>
-    <col min="20" max="20" width="16.7109375" customWidth="1"/>
+    <col min="11" max="12" width="20.85546875" customWidth="1"/>
+    <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.42578125" customWidth="1"/>
+    <col min="17" max="17" width="15.5703125" customWidth="1"/>
+    <col min="18" max="18" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.28515625" customWidth="1"/>
+    <col min="21" max="21" width="15" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -885,26 +961,30 @@
       <c r="I2" s="6"/>
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
-      <c r="L2" s="8"/>
+      <c r="L2" s="6"/>
       <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
+      <c r="N2" s="8"/>
       <c r="O2" s="6"/>
-      <c r="P2" s="7" t="s">
+      <c r="P2" s="6"/>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="6"/>
       <c r="S2" s="6"/>
       <c r="T2" s="6"/>
-      <c r="U2" s="8"/>
+      <c r="U2" s="6"/>
       <c r="V2" s="6"/>
-      <c r="W2" s="6" t="s">
+      <c r="W2" s="6"/>
+      <c r="X2" s="6"/>
+      <c r="Y2" s="8"/>
+      <c r="Z2" s="6"/>
+      <c r="AA2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="X2" s="6"/>
-      <c r="Y2" s="6"/>
+      <c r="AB2" s="6"/>
+      <c r="AC2" s="6"/>
     </row>
-    <row r="3" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -935,105 +1015,133 @@
       <c r="J3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="K3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="N3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="O3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="P3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="Q3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="R3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q3" s="2" t="s">
+      <c r="S3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="R3" s="3" t="s">
+      <c r="T3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="S3" s="2" t="s">
+      <c r="U3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="W3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="T3" s="3" t="s">
+      <c r="X3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="U3" s="9" t="s">
+      <c r="Y3" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="V3" s="1" t="s">
+      <c r="Z3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="W3" s="1" t="s">
+      <c r="AA3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="X3" s="1" t="s">
+      <c r="AB3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="Y3" s="1" t="s">
+      <c r="AC3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="I4" s="10"/>
       <c r="J4" s="10"/>
-      <c r="P4" s="10"/>
-      <c r="Q4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="R4" s="10"/>
+      <c r="S4" s="10"/>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="I6" s="10"/>
       <c r="J6" s="10"/>
-      <c r="P6" s="10"/>
-      <c r="Q6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="R6" s="10"/>
+      <c r="S6" s="10"/>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="I7" s="10"/>
       <c r="J7" s="10"/>
-      <c r="P7" s="10"/>
-      <c r="Q7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="R7" s="10"/>
+      <c r="S7" s="10"/>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="I8" s="10"/>
       <c r="J8" s="10"/>
-      <c r="P8" s="10"/>
-      <c r="Q8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="R8" s="10"/>
+      <c r="S8" s="10"/>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="I9" s="10"/>
       <c r="J9" s="10"/>
-      <c r="P9" s="10"/>
-      <c r="Q9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="R9" s="10"/>
+      <c r="S9" s="10"/>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="I10" s="10"/>
       <c r="J10" s="10"/>
-      <c r="P10" s="10"/>
-      <c r="Q10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="R10" s="10"/>
+      <c r="S10" s="10"/>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="K13" s="11"/>
-      <c r="L13" s="13"/>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="M13" s="11"/>
+      <c r="N13" s="13"/>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="J14" s="14"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="15"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="12"/>
+      <c r="N14" s="15"/>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="J15" s="14"/>
-      <c r="K15" s="12"/>
-      <c r="L15" s="13"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="12"/>
+      <c r="N15" s="13"/>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="K16" s="11"/>
-      <c r="L16" s="16"/>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="M16" s="11"/>
+      <c r="N16" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>